<commit_message>
Updated data for Dec 18
</commit_message>
<xml_diff>
--- a/andersonCountySC.xlsx
+++ b/andersonCountySC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidferrara/Documents/Clemson/The Tiger/COVID-19/Data/ttn-clemson-covid-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEBED10-42E9-C643-A722-DA61DB5F75CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C314649B-2D79-6E4B-A86A-3B28FFEFDCBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14360" windowHeight="16120" xr2:uid="{4AE96EF5-602B-A74E-86C2-19E719079597}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,6 +130,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -164,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -176,6 +183,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034DE182-6D63-5240-88C5-0C304C18E5A4}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -546,7 +554,7 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="D3" s="10">
-        <f t="shared" ref="D3:D41" si="0">(B3/202558)*100000</f>
+        <f t="shared" ref="D3:D42" si="0">(B3/202558)*100000</f>
         <v>4.4431718322653264</v>
       </c>
     </row>
@@ -558,7 +566,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="7">
-        <f t="shared" ref="C4:C41" si="1">(B4-B3)/B4</f>
+        <f t="shared" ref="C4:C42" si="1">(B4-B3)/B4</f>
         <v>0.5714285714285714</v>
       </c>
       <c r="D4" s="10">
@@ -1131,15 +1139,15 @@
         <v>44170</v>
       </c>
       <c r="B40">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C40" s="7">
         <f t="shared" si="1"/>
-        <v>0.32403718459495351</v>
+        <v>0.32493368700265252</v>
       </c>
       <c r="D40" s="10">
         <f t="shared" si="0"/>
-        <v>371.74537663286566</v>
+        <v>372.23906239200625</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1147,15 +1155,31 @@
         <v>44177</v>
       </c>
       <c r="B41">
-        <v>802</v>
+        <v>811</v>
       </c>
       <c r="C41" s="7">
         <f t="shared" si="1"/>
-        <v>6.1097256857855359E-2</v>
+        <v>7.0283600493218246E-2</v>
       </c>
       <c r="D41" s="10">
         <f t="shared" si="0"/>
-        <v>395.93597883075466</v>
+        <v>400.37915066302003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="11">
+        <v>44184</v>
+      </c>
+      <c r="B42">
+        <v>541</v>
+      </c>
+      <c r="C42" s="7">
+        <f t="shared" si="1"/>
+        <v>-0.49907578558225507</v>
+      </c>
+      <c r="D42" s="10">
+        <f t="shared" si="0"/>
+        <v>267.08399569506014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data for partial WE 1-9-21 and verified archived Clemson dash data for F2020
</commit_message>
<xml_diff>
--- a/andersonCountySC.xlsx
+++ b/andersonCountySC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidferrara/Documents/Clemson/The Tiger/COVID-19/Data/ttn-clemson-covid-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C314649B-2D79-6E4B-A86A-3B28FFEFDCBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D33E36-10DE-1F4B-B4C5-AE7ECD5E7622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14360" windowHeight="16120" xr2:uid="{4AE96EF5-602B-A74E-86C2-19E719079597}"/>
   </bookViews>
@@ -171,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -184,6 +184,7 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034DE182-6D63-5240-88C5-0C304C18E5A4}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1139,15 +1140,15 @@
         <v>44170</v>
       </c>
       <c r="B40">
-        <v>754</v>
+        <v>764</v>
       </c>
       <c r="C40" s="7">
         <f t="shared" si="1"/>
-        <v>0.32493368700265252</v>
+        <v>0.33376963350785338</v>
       </c>
       <c r="D40" s="10">
         <f t="shared" si="0"/>
-        <v>372.23906239200625</v>
+        <v>377.17591998341214</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1155,31 +1156,79 @@
         <v>44177</v>
       </c>
       <c r="B41">
-        <v>811</v>
+        <v>823</v>
       </c>
       <c r="C41" s="7">
         <f t="shared" si="1"/>
-        <v>7.0283600493218246E-2</v>
+        <v>7.168894289185905E-2</v>
       </c>
       <c r="D41" s="10">
         <f t="shared" si="0"/>
-        <v>400.37915066302003</v>
+        <v>406.3033797727071</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="11">
+      <c r="A42" s="12">
         <v>44184</v>
       </c>
       <c r="B42">
-        <v>541</v>
+        <v>997</v>
       </c>
       <c r="C42" s="7">
         <f t="shared" si="1"/>
-        <v>-0.49907578558225507</v>
+        <v>0.17452357071213642</v>
       </c>
       <c r="D42" s="10">
         <f t="shared" si="0"/>
-        <v>267.08399569506014</v>
+        <v>492.2047018631701</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2">
+        <v>44191</v>
+      </c>
+      <c r="B43">
+        <v>975</v>
+      </c>
+      <c r="C43" s="7">
+        <f t="shared" ref="C43:C45" si="2">(B43-B42)/B43</f>
+        <v>-2.2564102564102566E-2</v>
+      </c>
+      <c r="D43" s="10">
+        <f t="shared" ref="D43:D45" si="3">(B43/202558)*100000</f>
+        <v>481.34361516207707</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2">
+        <v>44198</v>
+      </c>
+      <c r="B44">
+        <v>1104</v>
+      </c>
+      <c r="C44" s="7">
+        <f t="shared" si="2"/>
+        <v>0.11684782608695653</v>
+      </c>
+      <c r="D44" s="10">
+        <f t="shared" si="3"/>
+        <v>545.02907809121336</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="11">
+        <v>44205</v>
+      </c>
+      <c r="B45">
+        <v>745</v>
+      </c>
+      <c r="C45" s="7">
+        <f t="shared" si="2"/>
+        <v>-0.48187919463087248</v>
+      </c>
+      <c r="D45" s="10">
+        <f t="shared" si="3"/>
+        <v>367.79589055974088</v>
       </c>
     </row>
   </sheetData>

</xml_diff>